<commit_message>
add indicator excel creation
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA4176E-03D6-4027-9E7C-1969123D7FBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F20AD10-CC88-4763-959D-1FEC4824B8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="892" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="892" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="活" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="922">
   <si>
     <t>General</t>
   </si>
@@ -3623,12 +3623,27 @@
     <t>git ,loop, indicator</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">trend: [False, 1, 1], pgain2: [True, 1, 1], </t>
+  </si>
+  <si>
+    <t>old wrong</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>new correct</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>best 2 combo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3773,14 +3788,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -3974,7 +3981,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4134,12 +4141,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4157,6 +4158,14 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5464,7 +5473,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.390625" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -5638,87 +5647,99 @@
       <c r="A17" s="52" t="s">
         <v>853</v>
       </c>
+      <c r="C17" s="52" t="s">
+        <v>920</v>
+      </c>
       <c r="D17" s="54"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A18" s="52" t="s">
         <v>852</v>
       </c>
-      <c r="D18" s="54"/>
+      <c r="C18" s="52" t="s">
+        <v>921</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A19" s="52" t="s">
         <v>854</v>
       </c>
-      <c r="C19" s="52" t="s">
-        <v>906</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>911</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A20" s="52" t="s">
         <v>855</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>906</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>904</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A21" s="52" t="s">
         <v>856</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>909</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>908</v>
-      </c>
+      <c r="D21" s="62"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.65">
       <c r="C22" s="52" t="s">
-        <v>907</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>905</v>
-      </c>
+        <v>919</v>
+      </c>
+      <c r="D22" s="62"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.65">
-      <c r="D23" s="55" t="s">
-        <v>857</v>
+      <c r="C23" s="52" t="s">
+        <v>906</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A24" s="52" t="s">
         <v>779</v>
       </c>
-      <c r="D24" s="56" t="s">
-        <v>789</v>
+      <c r="C24" s="52" t="s">
+        <v>906</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A25" s="52" t="s">
         <v>780</v>
       </c>
+      <c r="C25" s="52" t="s">
+        <v>909</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A26" s="52" t="s">
         <v>781</v>
       </c>
-      <c r="D26" s="54"/>
+      <c r="C26" s="52" t="s">
+        <v>907</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A27" s="52" t="s">
         <v>743</v>
       </c>
+      <c r="D27" s="64" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A28" s="52" t="s">
         <v>782</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.65">
@@ -11699,57 +11720,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.65">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="58" t="s">
         <v>721</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="62"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="60"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.65">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="56" t="s">
         <v>720</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="57" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="55" t="s">
         <v>719</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
       <c r="V2" s="51" t="s">
         <v>718</v>
       </c>

</xml_diff>

<commit_message>
changed backtest save to csv instead of excel to dramatically improve speed
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F20AD10-CC88-4763-959D-1FEC4824B8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E86FA80-7BAF-4013-AF49-75202BC80376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="892" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="949" activeTab="2" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="活" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="913">
   <si>
     <t>General</t>
   </si>
@@ -3416,10 +3416,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pri,fun,oth</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>used_on</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3432,18 +3428,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>asset_weight</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>date indicators=asset indicators+ derived date indicator</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>mot</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>class</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3500,57 +3488,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ts_code1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ts_code2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ts_code3</t>
-  </si>
-  <si>
-    <t>ts_code4</t>
-  </si>
-  <si>
-    <t>ts_code5</t>
-  </si>
-  <si>
-    <t>ts_code6</t>
-  </si>
-  <si>
-    <t>ts_code7</t>
-  </si>
-  <si>
-    <t>pearson1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>pearson2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>indicator pearson</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>indicator mean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>all ts_code view in general for all time until today</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>resistance calculation use numba</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -3636,6 +3573,38 @@
   </si>
   <si>
     <t>best 2 combo</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pri,fun,oth,date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>least square of error with trend</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pearson with future price</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean with future price</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>std with future price</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>trend with that</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>top n cased</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>top year</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4141,6 +4110,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4158,14 +4135,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5472,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B99DA0B-1B5F-4470-9FA3-A5DA13359AAE}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.390625" defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -5490,7 +5459,7 @@
         <v>777</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>900</v>
+        <v>883</v>
       </c>
       <c r="C1" s="52" t="s">
         <v>784</v>
@@ -5507,10 +5476,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A2" s="52" t="s">
-        <v>916</v>
+        <v>899</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>899</v>
+        <v>882</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>755</v>
@@ -5522,15 +5491,15 @@
         <v>749</v>
       </c>
       <c r="F2" s="52" t="s">
-        <v>915</v>
+        <v>898</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A3" s="52" t="s">
-        <v>917</v>
+        <v>900</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>901</v>
+        <v>884</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>753</v>
@@ -5585,7 +5554,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A8" s="52" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>849</v>
@@ -5596,7 +5565,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A9" s="52" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>859</v>
@@ -5607,7 +5576,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A10" s="52" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
       <c r="C10" s="52" t="s">
         <v>750</v>
@@ -5618,7 +5587,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A11" s="52" t="s">
-        <v>913</v>
+        <v>896</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>752</v>
@@ -5629,12 +5598,12 @@
         <v>850</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>910</v>
+        <v>893</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A13" s="52" t="s">
-        <v>914</v>
+        <v>897</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.65">
@@ -5648,7 +5617,7 @@
         <v>853</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>920</v>
+        <v>903</v>
       </c>
       <c r="D17" s="54"/>
     </row>
@@ -5657,10 +5626,10 @@
         <v>852</v>
       </c>
       <c r="C18" s="52" t="s">
-        <v>921</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>918</v>
+        <v>904</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>901</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.65">
@@ -5677,20 +5646,20 @@
       <c r="A21" s="52" t="s">
         <v>856</v>
       </c>
-      <c r="D21" s="62"/>
+      <c r="D21" s="56"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.65">
       <c r="C22" s="52" t="s">
-        <v>919</v>
-      </c>
-      <c r="D22" s="62"/>
+        <v>902</v>
+      </c>
+      <c r="D22" s="56"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.65">
       <c r="C23" s="52" t="s">
-        <v>906</v>
-      </c>
-      <c r="D23" s="63" t="s">
-        <v>911</v>
+        <v>889</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.65">
@@ -5698,10 +5667,10 @@
         <v>779</v>
       </c>
       <c r="C24" s="52" t="s">
-        <v>906</v>
-      </c>
-      <c r="D24" s="63" t="s">
-        <v>904</v>
+        <v>889</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.65">
@@ -5709,10 +5678,10 @@
         <v>780</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>909</v>
-      </c>
-      <c r="D25" s="63" t="s">
-        <v>908</v>
+        <v>892</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>891</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.65">
@@ -5720,17 +5689,17 @@
         <v>781</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>907</v>
-      </c>
-      <c r="D26" s="63" t="s">
-        <v>905</v>
+        <v>890</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A27" s="52" t="s">
         <v>743</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="58" t="s">
         <v>857</v>
       </c>
     </row>
@@ -5738,7 +5707,7 @@
       <c r="A28" s="52" t="s">
         <v>782</v>
       </c>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="58" t="s">
         <v>789</v>
       </c>
     </row>
@@ -8877,7 +8846,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -9772,10 +9741,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540D9E59-6473-4377-9563-7805E5BAFFF1}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -9785,168 +9754,143 @@
     <col min="5" max="5" width="11.60546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A1" t="s">
         <v>863</v>
       </c>
       <c r="B1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
-        <v>868</v>
-      </c>
-      <c r="F1" t="s">
-        <v>870</v>
-      </c>
-      <c r="K1" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.65">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="J3" t="s">
-        <v>894</v>
-      </c>
-      <c r="K3" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="I4" t="s">
-        <v>885</v>
-      </c>
-      <c r="J4" t="s">
-        <v>892</v>
-      </c>
-      <c r="K4" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A5" t="s">
         <v>863</v>
       </c>
-      <c r="I5" t="s">
-        <v>886</v>
-      </c>
-      <c r="J5" t="s">
-        <v>893</v>
-      </c>
-      <c r="K5" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.65">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A6" t="s">
         <v>113</v>
       </c>
       <c r="B6" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A7" t="s">
         <v>864</v>
       </c>
-      <c r="I6" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>865</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A8" t="s">
         <v>866</v>
       </c>
-      <c r="I7" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="A8" t="s">
-        <v>867</v>
-      </c>
-      <c r="I8" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.65">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A9" t="s">
-        <v>878</v>
-      </c>
-      <c r="I9" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="I10" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.65">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A11" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A12" t="s">
+        <v>870</v>
+      </c>
+      <c r="B12" t="s">
+        <v>871</v>
+      </c>
+      <c r="D12" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A13" t="s">
         <v>873</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>874</v>
       </c>
-      <c r="D12" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="A13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A14" t="s">
         <v>876</v>
-      </c>
-      <c r="B13" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="A14" t="s">
-        <v>879</v>
       </c>
       <c r="B14">
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.65">
       <c r="A15" t="s">
+        <v>877</v>
+      </c>
+      <c r="B15" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A16" t="s">
+        <v>879</v>
+      </c>
+      <c r="B16" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="A17" t="s">
         <v>880</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="A18" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.65">
-      <c r="A16" t="s">
-        <v>882</v>
-      </c>
-      <c r="B16" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A17" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.65">
-      <c r="A18" t="s">
-        <v>884</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="B21" t="s">
+        <v>906</v>
+      </c>
+      <c r="C21" t="s">
+        <v>907</v>
+      </c>
+      <c r="D21" t="s">
+        <v>908</v>
+      </c>
+      <c r="E21" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="A22" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="A23" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="A24" t="s">
+        <v>912</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.65">
       <c r="A37" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
   </sheetData>
@@ -9960,7 +9904,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -11720,57 +11664,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.65">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>721</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.65">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="60" t="s">
         <v>720</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="55" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="59" t="s">
         <v>719</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
       <c r="V2" s="51" t="s">
         <v>718</v>
       </c>

</xml_diff>

<commit_message>
add portfolio money part 1
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C573B7-860D-43CF-BA1F-F3A53A0AD7EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE7974-BB08-432D-998C-6ADC04C64557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25611" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="未做" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="843">
   <si>
     <t>General</t>
   </si>
@@ -3209,6 +3209,90 @@
   </si>
   <si>
     <t>科创板，新三板，港股，德股，美股</t>
+  </si>
+  <si>
+    <t>finish implement portfolio capital cash, weight, fee</t>
+  </si>
+  <si>
+    <t>day2</t>
+  </si>
+  <si>
+    <t>day1</t>
+  </si>
+  <si>
+    <t>day3</t>
+  </si>
+  <si>
+    <t>day4</t>
+  </si>
+  <si>
+    <t>day5</t>
+  </si>
+  <si>
+    <t>day6</t>
+  </si>
+  <si>
+    <t>day7</t>
+  </si>
+  <si>
+    <t>day8</t>
+  </si>
+  <si>
+    <t>day9</t>
+  </si>
+  <si>
+    <t>day10</t>
+  </si>
+  <si>
+    <t>day11</t>
+  </si>
+  <si>
+    <t>day12</t>
+  </si>
+  <si>
+    <t>day13</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>hold</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>ts_code</t>
+  </si>
+  <si>
+    <t>everything else</t>
+  </si>
+  <si>
+    <t>day1,sell,ts_code</t>
+  </si>
+  <si>
+    <t>day1,hold,ts_code</t>
+  </si>
+  <si>
+    <t>dict_dict</t>
+  </si>
+  <si>
+    <t>dict_a</t>
+  </si>
+  <si>
+    <t>for each setting</t>
+  </si>
+  <si>
+    <t>for each day</t>
+  </si>
+  <si>
+    <t>for each trade type</t>
+  </si>
+  <si>
+    <t>sold</t>
+  </si>
+  <si>
+    <t>buy 8</t>
   </si>
 </sst>
 </file>
@@ -3682,12 +3766,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4994,8 +5078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B99DA0B-1B5F-4470-9FA3-A5DA13359AAE}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.54296875" defaultRowHeight="14.75"/>
@@ -5064,6 +5148,9 @@
       <c r="A4" t="s">
         <v>710</v>
       </c>
+      <c r="B4" s="49" t="s">
+        <v>815</v>
+      </c>
       <c r="E4" s="49" t="s">
         <v>682</v>
       </c>
@@ -5229,7 +5316,7 @@
       <c r="C19" s="49" t="s">
         <v>709</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="56" t="s">
         <v>803</v>
       </c>
     </row>
@@ -5275,8 +5362,148 @@
     <row r="26" spans="1:6">
       <c r="F26" s="54"/>
     </row>
-    <row r="49" spans="2:2">
+    <row r="27" spans="1:6">
+      <c r="C27" s="49" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28" s="49" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="E29" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31" s="49" t="s">
+        <v>839</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>841</v>
+      </c>
+      <c r="E31" s="49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32" s="49" t="s">
+        <v>838</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>830</v>
+      </c>
+      <c r="E32" s="49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="49" t="s">
+        <v>840</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>830</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="C36" s="49" t="s">
+        <v>836</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="C37" s="49" t="s">
+        <v>817</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>829</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" s="49" t="s">
+        <v>816</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>830</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>832</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="C39" s="49" t="s">
+        <v>818</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="C40" s="49" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="C41" s="49" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="C42" s="49" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="C43" s="49" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="C44" s="49" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="C45" s="49" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="C46" s="49" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="C47" s="49" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="C48" s="49" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
       <c r="B49"/>
+      <c r="C49" s="49" t="s">
+        <v>828</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5671,14 +5898,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
         <v>805</v>
       </c>
-      <c r="E1" s="56"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
@@ -5766,29 +5993,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>717</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58" t="s">
         <v>723</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56" t="s">
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58" t="s">
         <v>724</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
@@ -5821,10 +6048,10 @@
       <c r="J2" t="s">
         <v>752</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="58" t="s">
         <v>764</v>
       </c>
-      <c r="L2" s="56"/>
+      <c r="L2" s="58"/>
       <c r="M2" t="s">
         <v>759</v>
       </c>
@@ -11672,7 +11899,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="57" t="s">
         <v>606</v>
       </c>
     </row>
@@ -11685,7 +11912,7 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="57" t="s">
         <v>811</v>
       </c>
     </row>

</xml_diff>

<commit_message>
support and resistance 2
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79FF48-26A0-4DF9-8496-3B4950B62252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF29FA4-0CDE-4F83-9DAA-47E4E5D9FE2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25611" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
@@ -5093,7 +5093,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.54296875" defaultRowHeight="14.75"/>
@@ -5124,9 +5124,6 @@
       <c r="A2" s="49" t="s">
         <v>693</v>
       </c>
-      <c r="B2" t="s">
-        <v>703</v>
-      </c>
       <c r="C2" s="49" t="s">
         <v>795</v>
       </c>
@@ -5138,9 +5135,6 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>705</v>
-      </c>
       <c r="C3" s="49" t="s">
         <v>799</v>
       </c>
@@ -5152,8 +5146,8 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="B4" s="49" t="s">
-        <v>778</v>
+      <c r="C4" s="56" t="s">
+        <v>794</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>677</v>
@@ -5163,9 +5157,6 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" s="49" t="s">
-        <v>779</v>
-      </c>
       <c r="D5" s="49" t="s">
         <v>797</v>
       </c>
@@ -5177,9 +5168,6 @@
       <c r="A6" s="49" t="s">
         <v>688</v>
       </c>
-      <c r="B6" s="49" t="s">
-        <v>780</v>
-      </c>
       <c r="D6" s="49" t="s">
         <v>702</v>
       </c>
@@ -5188,9 +5176,6 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="49" t="s">
-        <v>781</v>
-      </c>
       <c r="D7" s="49" t="s">
         <v>675</v>
       </c>
@@ -5306,7 +5291,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="49" t="s">
         <v>701</v>
       </c>
@@ -5317,35 +5302,84 @@
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="B18" s="49" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="C19" s="56" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="E20" s="52"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="E21" s="53"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="E22" s="53"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="53"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="E24" s="53"/>
-    </row>
-    <row r="25" spans="1:5">
+    <row r="21" spans="1:6">
+      <c r="B21" t="s">
+        <v>703</v>
+      </c>
+      <c r="D21" s="49">
+        <v>1</v>
+      </c>
+      <c r="E21" s="53">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F21">
+        <f>E21*1000</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="s">
+        <v>705</v>
+      </c>
+      <c r="D22" s="49">
+        <v>1</v>
+      </c>
+      <c r="E22" s="53">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F24" si="0">E22*1000</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" s="49" t="s">
+        <v>778</v>
+      </c>
+      <c r="D23" s="49">
+        <v>2</v>
+      </c>
+      <c r="E23" s="53">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" s="49" t="s">
+        <v>779</v>
+      </c>
+      <c r="D24" s="49">
+        <v>3</v>
+      </c>
+      <c r="E24" s="53">
+        <v>0.44</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" s="49" t="s">
+        <v>780</v>
+      </c>
       <c r="E25" s="54"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
+      <c r="B26" s="49" t="s">
+        <v>781</v>
+      </c>
       <c r="E26" s="54"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support and resistance fine tune
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF29FA4-0CDE-4F83-9DAA-47E4E5D9FE2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8C0E5B-99F7-4821-9443-296BB0B94183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25611" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="未做" sheetId="10" r:id="rId1"/>
-    <sheet name="kelly" sheetId="19" r:id="rId2"/>
-    <sheet name="Calc" sheetId="18" r:id="rId3"/>
-    <sheet name="测试" sheetId="17" r:id="rId4"/>
-    <sheet name="信号" sheetId="15" r:id="rId5"/>
-    <sheet name="问答" sheetId="1" r:id="rId6"/>
-    <sheet name="指标" sheetId="9" r:id="rId7"/>
-    <sheet name="科学" sheetId="6" r:id="rId8"/>
-    <sheet name="经济" sheetId="5" r:id="rId9"/>
-    <sheet name="储存" sheetId="3" r:id="rId10"/>
-    <sheet name="数据" sheetId="7" r:id="rId11"/>
-    <sheet name="Meta" sheetId="2" r:id="rId12"/>
+    <sheet name="模拟" sheetId="20" r:id="rId2"/>
+    <sheet name="kelly" sheetId="19" r:id="rId3"/>
+    <sheet name="Calc" sheetId="18" r:id="rId4"/>
+    <sheet name="测试" sheetId="17" r:id="rId5"/>
+    <sheet name="信号" sheetId="15" r:id="rId6"/>
+    <sheet name="问答" sheetId="1" r:id="rId7"/>
+    <sheet name="指标" sheetId="9" r:id="rId8"/>
+    <sheet name="科学" sheetId="6" r:id="rId9"/>
+    <sheet name="经济" sheetId="5" r:id="rId10"/>
+    <sheet name="储存" sheetId="3" r:id="rId11"/>
+    <sheet name="数据" sheetId="7" r:id="rId12"/>
+    <sheet name="Meta" sheetId="2" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">问答!$A$1:$F$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">问答!$A$1:$F$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="858">
   <si>
     <t>General</t>
   </si>
@@ -3183,78 +3184,6 @@
     <t>close price</t>
   </si>
   <si>
-    <t>300454.SZ</t>
-  </si>
-  <si>
-    <t>深信服</t>
-  </si>
-  <si>
-    <t>601222.SH</t>
-  </si>
-  <si>
-    <t>林洋能源</t>
-  </si>
-  <si>
-    <t>000637.SZ</t>
-  </si>
-  <si>
-    <t>茂化实华</t>
-  </si>
-  <si>
-    <t>600220.SH</t>
-  </si>
-  <si>
-    <t>江苏阳光</t>
-  </si>
-  <si>
-    <t>002129.SZ</t>
-  </si>
-  <si>
-    <t>中环股份</t>
-  </si>
-  <si>
-    <t>002065.SZ</t>
-  </si>
-  <si>
-    <t>东华软件</t>
-  </si>
-  <si>
-    <t>000815.SZ</t>
-  </si>
-  <si>
-    <t>美利云</t>
-  </si>
-  <si>
-    <t>002298.SZ</t>
-  </si>
-  <si>
-    <t>中电兴发</t>
-  </si>
-  <si>
-    <t>002912.SZ</t>
-  </si>
-  <si>
-    <t>中新赛克</t>
-  </si>
-  <si>
-    <t>600986.SH</t>
-  </si>
-  <si>
-    <t>科达股份</t>
-  </si>
-  <si>
-    <t>603185.SH</t>
-  </si>
-  <si>
-    <t>上机数控</t>
-  </si>
-  <si>
-    <t>300111.SZ</t>
-  </si>
-  <si>
-    <t>向日葵</t>
-  </si>
-  <si>
     <t>shares to buy</t>
   </si>
   <si>
@@ -3307,6 +3236,102 @@
   </si>
   <si>
     <t>use particial regression = observe stock price under different condition and then use regression</t>
+  </si>
+  <si>
+    <t>603229.SH</t>
+  </si>
+  <si>
+    <t>奥翔药业</t>
+  </si>
+  <si>
+    <t>002221.SZ</t>
+  </si>
+  <si>
+    <t>东华能源</t>
+  </si>
+  <si>
+    <t>trade_date</t>
+  </si>
+  <si>
+    <t>simu</t>
+  </si>
+  <si>
+    <t>maxsize</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>600448.SH</t>
+  </si>
+  <si>
+    <t>华纺股份</t>
+  </si>
+  <si>
+    <t>000078.SZ</t>
+  </si>
+  <si>
+    <t>海王生物</t>
+  </si>
+  <si>
+    <t>000518.SZ</t>
+  </si>
+  <si>
+    <t>四环生物</t>
+  </si>
+  <si>
+    <t>600156.SH</t>
+  </si>
+  <si>
+    <t>华升股份</t>
+  </si>
+  <si>
+    <t>002341.SZ</t>
+  </si>
+  <si>
+    <t>新纶科技</t>
+  </si>
+  <si>
+    <t>300266.SZ</t>
+  </si>
+  <si>
+    <t>兴源环境</t>
+  </si>
+  <si>
+    <t>000949.SZ</t>
+  </si>
+  <si>
+    <t>新乡化纤</t>
+  </si>
+  <si>
+    <t>002551.SZ</t>
+  </si>
+  <si>
+    <t>尚荣医疗</t>
+  </si>
+  <si>
+    <t>002332.SZ</t>
+  </si>
+  <si>
+    <t>仙琚制药</t>
+  </si>
+  <si>
+    <t>600636.SH</t>
+  </si>
+  <si>
+    <t>三爱富</t>
+  </si>
+  <si>
+    <t>what about date fgain if 90% stocks winning and mean pct_chg is 2%</t>
+  </si>
+  <si>
+    <t>rsi cross over</t>
+  </si>
+  <si>
+    <t>autoregression not on plain pct_chg , but on smoothed ma pct_chg</t>
+  </si>
+  <si>
+    <t>52week high and low for fgain</t>
   </si>
 </sst>
 </file>
@@ -5093,7 +5118,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.54296875" defaultRowHeight="14.75"/>
@@ -5135,6 +5160,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
+      <c r="A3" s="49" t="s">
+        <v>855</v>
+      </c>
       <c r="C3" s="49" t="s">
         <v>799</v>
       </c>
@@ -5146,6 +5174,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
+      <c r="A4" s="49" t="s">
+        <v>856</v>
+      </c>
       <c r="C4" s="56" t="s">
         <v>794</v>
       </c>
@@ -5157,6 +5188,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
+      <c r="A5" s="49" t="s">
+        <v>857</v>
+      </c>
       <c r="D5" s="49" t="s">
         <v>797</v>
       </c>
@@ -5184,6 +5218,9 @@
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" s="49" t="s">
+        <v>854</v>
+      </c>
       <c r="D8" s="49" t="s">
         <v>764</v>
       </c>
@@ -5246,7 +5283,7 @@
         <v>769</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>847</v>
+        <v>823</v>
       </c>
       <c r="E13" s="51" t="s">
         <v>802</v>
@@ -5260,7 +5297,7 @@
         <v>770</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>848</v>
+        <v>824</v>
       </c>
       <c r="E14" s="49" t="s">
         <v>692</v>
@@ -5288,7 +5325,7 @@
         <v>772</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>849</v>
+        <v>825</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5399,6 +5436,252 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8E847-F0F5-4AC0-A22C-A661CAF5EEE3}">
+  <dimension ref="A1:A83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>447</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE354621-588A-4B21-BB13-B5E3178F81D7}">
   <dimension ref="A1:L226"/>
   <sheetViews>
@@ -8068,7 +8351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAE67A0-59E8-4407-9000-5ED3F9ACE7BD}">
   <dimension ref="A1:J18"/>
   <sheetViews>
@@ -8403,7 +8686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001E9E6C-9755-494E-B35F-D95B93657434}">
   <dimension ref="A1:E72"/>
   <sheetViews>
@@ -8767,6 +9050,63 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A95E259-184D-4CA8-9B8B-55931C83A92B}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>20200217</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>3.19</v>
+      </c>
+      <c r="D2">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>20200217</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2.4</v>
+      </c>
+      <c r="D3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46AC116-74D7-4096-87CF-7429FB535D3B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -8781,10 +9121,10 @@
         <v>0.91</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>836</v>
+        <v>812</v>
       </c>
       <c r="C1" t="s">
-        <v>841</v>
+        <v>817</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8792,10 +9132,10 @@
         <v>0.01</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>837</v>
+        <v>813</v>
       </c>
       <c r="C2" t="s">
-        <v>842</v>
+        <v>818</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8803,10 +9143,10 @@
         <v>0.03</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>838</v>
+        <v>814</v>
       </c>
       <c r="C3" t="s">
-        <v>843</v>
+        <v>819</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8820,7 +9160,7 @@
       </c>
       <c r="B5" s="49"/>
       <c r="C5" t="s">
-        <v>844</v>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -8828,233 +9168,233 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74848AFD-2D90-41D5-97CC-2C0F39AA2810}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
-    <col min="3" max="3" width="12.40625" customWidth="1"/>
-    <col min="4" max="4" width="14.40625" customWidth="1"/>
+    <col min="1" max="1" width="14.40625" customWidth="1"/>
+    <col min="4" max="4" width="12.40625" customWidth="1"/>
     <col min="11" max="11" width="11.58984375" customWidth="1"/>
     <col min="12" max="12" width="11.04296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B1" t="s">
         <v>804</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>806</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>807</v>
       </c>
-      <c r="D1" t="s">
-        <v>832</v>
-      </c>
       <c r="E1" t="s">
-        <v>833</v>
+        <v>809</v>
       </c>
       <c r="H1" t="s">
         <v>805</v>
       </c>
       <c r="I1">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="J1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <f t="shared" ref="A2:A13" si="0">ROUND($I$1/$I$2/D2,0)</f>
+        <v>43</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>826</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>827</v>
+      </c>
+      <c r="D2" s="25">
+        <v>193.98003992015899</v>
+      </c>
+      <c r="I2">
+        <f>COUNTA(B1:B2000)-1</f>
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>1603</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>828</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>829</v>
+      </c>
+      <c r="D3" s="25">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>1766</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>834</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
-        <v>808</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>809</v>
-      </c>
-      <c r="C2" s="25">
-        <v>37.65</v>
-      </c>
-      <c r="D2">
-        <f>ROUND($I$1/$I$2/C2,0)</f>
-        <v>22</v>
-      </c>
-      <c r="I2">
-        <f>COUNTA(A1:A2000)-1</f>
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="25" t="s">
-        <v>810</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>811</v>
-      </c>
-      <c r="C3" s="25">
-        <v>15.2799964215423</v>
-      </c>
-      <c r="D3">
-        <f>ROUND($I$1/$I$2/C3,0)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="25" t="s">
-        <v>812</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>813</v>
-      </c>
-      <c r="C4" s="25">
-        <v>44.3599992274114</v>
-      </c>
-      <c r="D4">
-        <f>ROUND($I$1/$I$2/C4,0)</f>
-        <v>19</v>
+      <c r="D4" s="25">
+        <v>4.7199976107991803</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="25" t="s">
-        <v>814</v>
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3516</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>815</v>
-      </c>
-      <c r="C5" s="25">
-        <v>22.9499755501222</v>
-      </c>
-      <c r="D5">
-        <f>ROUND($I$1/$I$2/C5,0)</f>
-        <v>36</v>
+        <v>836</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>837</v>
+      </c>
+      <c r="D5" s="25">
+        <v>2.3700011782726502</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="25" t="s">
-        <v>816</v>
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>489</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>817</v>
-      </c>
-      <c r="C6" s="25">
-        <v>7.2700020012007203</v>
-      </c>
-      <c r="D6">
-        <f>ROUND($I$1/$I$2/C6,0)</f>
-        <v>115</v>
+        <v>838</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>839</v>
+      </c>
+      <c r="D6" s="25">
+        <v>17.050011851149499</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="25" t="s">
-        <v>818</v>
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>534</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>819</v>
-      </c>
-      <c r="C7" s="25">
-        <v>7.24</v>
-      </c>
-      <c r="D7">
-        <f>ROUND($I$1/$I$2/C7,0)</f>
-        <v>115</v>
+        <v>840</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="D7" s="25">
+        <v>15.6</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="25" t="s">
-        <v>820</v>
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1107</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>821</v>
-      </c>
-      <c r="C8" s="25">
-        <v>66.459994932860397</v>
-      </c>
-      <c r="D8">
-        <f>ROUND($I$1/$I$2/C8,0)</f>
-        <v>13</v>
+        <v>842</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>843</v>
+      </c>
+      <c r="D8" s="25">
+        <v>7.5300058038305204</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="25" t="s">
-        <v>822</v>
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>875</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>823</v>
-      </c>
-      <c r="C9" s="25">
-        <v>34.4</v>
-      </c>
-      <c r="D9">
-        <f>ROUND($I$1/$I$2/C9,0)</f>
-        <v>24</v>
+        <v>844</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>845</v>
+      </c>
+      <c r="D9" s="25">
+        <v>9.5199871671478995</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="25" t="s">
-        <v>824</v>
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>825</v>
-      </c>
-      <c r="C10" s="25">
-        <v>6.5</v>
-      </c>
-      <c r="D10">
-        <f>ROUND($I$1/$I$2/C10,0)</f>
-        <v>128</v>
+        <v>846</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="D10" s="25">
+        <v>178.89999999999901</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="25" t="s">
-        <v>826</v>
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1952</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>827</v>
-      </c>
-      <c r="C11" s="25">
-        <v>1.86000530785562</v>
-      </c>
-      <c r="D11">
-        <f>ROUND($I$1/$I$2/C11,0)</f>
-        <v>448</v>
+        <v>848</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>849</v>
+      </c>
+      <c r="D11" s="25">
+        <v>4.2699914015477196</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="25" t="s">
-        <v>828</v>
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>204</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>829</v>
-      </c>
-      <c r="C12" s="25">
-        <v>30.6</v>
-      </c>
-      <c r="D12">
-        <f>ROUND($I$1/$I$2/C12,0)</f>
-        <v>27</v>
+        <v>850</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>851</v>
+      </c>
+      <c r="D12" s="25">
+        <v>40.9</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="25" t="s">
-        <v>830</v>
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>3671</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>831</v>
-      </c>
-      <c r="C13" s="25">
-        <v>18.679984301412802</v>
-      </c>
-      <c r="D13">
-        <f>ROUND($I$1/$I$2/C13,0)</f>
-        <v>45</v>
+        <v>852</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>853</v>
+      </c>
+      <c r="D13" s="25">
+        <v>2.2700089126559702</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -9066,7 +9406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7DADBA-5C62-4A34-AC9B-233ED54E173D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -9156,7 +9496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7146CF-7905-411D-AB60-014FE18FF5ED}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
@@ -9443,7 +9783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D688AAC-D99D-48A3-AA61-E482F3E85832}">
   <dimension ref="A1:E66"/>
   <sheetViews>
@@ -10386,20 +10726,20 @@
       <c r="B56" s="21"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19" t="s">
-        <v>839</v>
+        <v>815</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>840</v>
+        <v>816</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19" t="s">
-        <v>845</v>
+        <v>821</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>846</v>
+        <v>822</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -10492,7 +10832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C00FA0-CF19-4FFB-9491-FC2DC5B84460}">
   <dimension ref="A1:G64"/>
   <sheetViews>
@@ -11028,7 +11368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32841ADC-F22B-4401-BCBA-6E5CDCC57F2A}">
   <dimension ref="A1:D100"/>
   <sheetViews>
@@ -11868,250 +12208,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8E847-F0F5-4AC0-A22C-A661CAF5EEE3}">
-  <dimension ref="A1:A83"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>447</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
support and resistance fine tune 2
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8C0E5B-99F7-4821-9443-296BB0B94183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B3C97-D7CB-4EBB-BDB0-986204D61EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25611" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="844" activeTab="3" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="未做" sheetId="10" r:id="rId1"/>
@@ -5117,7 +5117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B99DA0B-1B5F-4470-9FA3-A5DA13359AAE}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -9172,8 +9172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74848AFD-2D90-41D5-97CC-2C0F39AA2810}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -9213,7 +9213,7 @@
     <row r="2" spans="1:10">
       <c r="A2">
         <f t="shared" ref="A2:A13" si="0">ROUND($I$1/$I$2/D2,0)</f>
-        <v>43</v>
+        <v>298</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>826</v>
@@ -9222,7 +9222,7 @@
         <v>827</v>
       </c>
       <c r="D2" s="25">
-        <v>193.98003992015899</v>
+        <v>27.939980158730101</v>
       </c>
       <c r="I2">
         <f>COUNTA(B1:B2000)-1</f>
@@ -9235,7 +9235,7 @@
     <row r="3" spans="1:10">
       <c r="A3">
         <f t="shared" si="0"/>
-        <v>1603</v>
+        <v>914</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>828</v>
@@ -9244,13 +9244,13 @@
         <v>829</v>
       </c>
       <c r="D3" s="25">
-        <v>5.2</v>
+        <v>9.1199999999999992</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
         <f t="shared" si="0"/>
-        <v>1766</v>
+        <v>1558</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>834</v>
@@ -9259,13 +9259,13 @@
         <v>835</v>
       </c>
       <c r="D4" s="25">
-        <v>4.7199976107991803</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>3516</v>
+        <v>1587</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>836</v>
@@ -9274,13 +9274,13 @@
         <v>837</v>
       </c>
       <c r="D5" s="25">
-        <v>2.3700011782726502</v>
+        <v>5.2499999999999902</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>489</v>
+        <v>1465</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>838</v>
@@ -9289,13 +9289,13 @@
         <v>839</v>
       </c>
       <c r="D6" s="25">
-        <v>17.050011851149499</v>
+        <v>5.6899964187656602</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>534</v>
+        <v>1881</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>840</v>
@@ -9304,13 +9304,13 @@
         <v>841</v>
       </c>
       <c r="D7" s="25">
-        <v>15.6</v>
+        <v>4.42999472851871</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>1107</v>
+        <v>1233</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>842</v>
@@ -9319,13 +9319,13 @@
         <v>843</v>
       </c>
       <c r="D8" s="25">
-        <v>7.5300058038305204</v>
+        <v>6.7599951917297698</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>875</v>
+        <v>2033</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>844</v>
@@ -9334,13 +9334,13 @@
         <v>845</v>
       </c>
       <c r="D9" s="25">
-        <v>9.5199871671478995</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>2210</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>846</v>
@@ -9349,13 +9349,13 @@
         <v>847</v>
       </c>
       <c r="D10" s="25">
-        <v>178.89999999999901</v>
+        <v>3.7699936695505301</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>1952</v>
+        <v>1296</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>848</v>
@@ -9364,13 +9364,13 @@
         <v>849</v>
       </c>
       <c r="D11" s="25">
-        <v>4.2699914015477196</v>
+        <v>6.43000361054278</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>814</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>850</v>
@@ -9379,13 +9379,13 @@
         <v>851</v>
       </c>
       <c r="D12" s="25">
-        <v>40.9</v>
+        <v>10.240007883326699</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>3671</v>
+        <v>622</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>852</v>
@@ -9394,7 +9394,7 @@
         <v>853</v>
       </c>
       <c r="D13" s="25">
-        <v>2.2700089126559702</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="14" spans="1:10">

</xml_diff>

<commit_message>
support and resistance fine tune 4
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191B3C97-D7CB-4EBB-BDB0-986204D61EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6F5CFE-BB81-4C27-86A9-6F9124A02AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="844" activeTab="3" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="未做" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="859">
   <si>
     <t>General</t>
   </si>
@@ -3332,6 +3332,9 @@
   </si>
   <si>
     <t>52week high and low for fgain</t>
+  </si>
+  <si>
+    <t>use support resistance on volume and other indicator</t>
   </si>
 </sst>
 </file>
@@ -5117,8 +5120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B99DA0B-1B5F-4470-9FA3-A5DA13359AAE}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.54296875" defaultRowHeight="14.75"/>
@@ -5210,6 +5213,9 @@
       </c>
     </row>
     <row r="7" spans="1:5">
+      <c r="A7" s="49" t="s">
+        <v>858</v>
+      </c>
       <c r="D7" s="49" t="s">
         <v>675</v>
       </c>
@@ -9172,8 +9178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74848AFD-2D90-41D5-97CC-2C0F39AA2810}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>

</xml_diff>

<commit_message>
support and resistance fine tune 5
</commit_message>
<xml_diff>
--- a/All-In-One.xlsx
+++ b/All-In-One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\私人\私人 Stock 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6F5CFE-BB81-4C27-86A9-6F9124A02AD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693C3800-285B-47C6-BE52-96C3EE6E511B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="15180" windowHeight="9580" tabRatio="844" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
+    <workbookView xWindow="25611" yWindow="-103" windowWidth="16663" windowHeight="9463" tabRatio="844" activeTab="1" xr2:uid="{E5341D75-8C28-4386-8249-C2E39010DE6C}"/>
   </bookViews>
   <sheets>
     <sheet name="未做" sheetId="10" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="864">
   <si>
     <t>General</t>
   </si>
@@ -3335,6 +3335,21 @@
   </si>
   <si>
     <t>use support resistance on volume and other indicator</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>plain indicator fgain pearson</t>
+  </si>
+  <si>
+    <t>apply resistance, then fgain pearson</t>
+  </si>
+  <si>
+    <t>apply rsi, then fgain pearson</t>
+  </si>
+  <si>
+    <t>apply trend, then fgain pearson</t>
   </si>
 </sst>
 </file>
@@ -5120,8 +5135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B99DA0B-1B5F-4470-9FA3-A5DA13359AAE}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.54296875" defaultRowHeight="14.75"/>
@@ -9059,11 +9074,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A95E259-184D-4CA8-9B8B-55931C83A92B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
+  <cols>
+    <col min="1" max="1" width="11.76953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -9507,7 +9525,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75"/>
@@ -9766,14 +9784,52 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="13" spans="1:17">
+      <c r="E13" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>759</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>